<commit_message>
updating documentation and input files
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
   <si>
     <t xml:space="preserve">Access </t>
   </si>
@@ -39,36 +39,6 @@
   </si>
   <si>
     <t>Based on data for the years 2016-2018</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Open Access, Accessed </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>XXXx</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Office for National Statistics,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> link :</t>
-    </r>
   </si>
   <si>
     <t>https://www.ons.gov.uk/peoplepopulationandcommunity/birthsdeathsandmarriages/deaths/datasets/weeklyprovisionalfiguresondeathsregisteredinenglandandwales</t>
@@ -88,40 +58,112 @@
     </r>
   </si>
   <si>
-    <t>UK_covid19</t>
-  </si>
-  <si>
-    <t>Deaths from covid19 in the UK by age group</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov/nchs/nvss/vsrr/covid19/index.htm</t>
-  </si>
-  <si>
     <t>Open access, Accessed: April 29, 2020</t>
   </si>
   <si>
-    <t>US_covid19</t>
-  </si>
-  <si>
-    <t>Deaths from covid19 in the US by age group</t>
-  </si>
-  <si>
-    <t>Life Tables for US males</t>
-  </si>
-  <si>
     <t>SOURCE: NCHS, National Vital Statistics System, Mortality.</t>
   </si>
   <si>
-    <t>UK q(x)</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Life Tables for UK </t>
-  </si>
-  <si>
-    <t>US q(x)</t>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>male_LT &amp; female_LT</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Life Tables for US</t>
+  </si>
+  <si>
+    <t>Life Tables for Canada</t>
+  </si>
+  <si>
+    <t>https://www150.statcan.gc.ca/n1/pub/84-537-x/84-537-x2019002-eng.htm</t>
+  </si>
+  <si>
+    <t>Life Tables, Canada, Provinces and Territories 1980/1982 to 2016/2018</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Office for National Statistics</t>
+  </si>
+  <si>
+    <t>Life Tables for Norway</t>
+  </si>
+  <si>
+    <t>Life Tables for Israel</t>
+  </si>
+  <si>
+    <t>07902: Life tables, by age x, year, sex and contents</t>
+  </si>
+  <si>
+    <t>Open Access, Last accessed April 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cdc.gov/nchs/nvss/vsrr/covid19/index.htm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssb.no/en </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cbs.gov.il/en/publications/Pages/2019/Complete-Life-Tables-Of-Israel%20-%202013-2017.aspx#losExcelos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete Life Tables Of Israel - 2013-2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths registered weekly in England and Wales, provisional </t>
+  </si>
+  <si>
+    <t>Provisional Death Counts for Coronavirus Disease (COVID-19)</t>
+  </si>
+  <si>
+    <t>age_covid</t>
+  </si>
+  <si>
+    <t>Deaths from covid19 by age group</t>
+  </si>
+  <si>
+    <t>https://www.canada.ca/content/dam/phac-aspc/documents/services/diseases/2019-novel-coronavirus-infection/surv-covid19-epi-update-eng.pdf</t>
+  </si>
+  <si>
+    <t>To be added</t>
+  </si>
+  <si>
+    <t>CORONAVIRUS DISEASE 2019 (COVID-19) DAILY UPDATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.04.22-dagsrapport-covid-19.pdf </t>
+  </si>
+  <si>
+    <t>COVID-19 Dagsrapport</t>
+  </si>
+  <si>
+    <t>qol_norm</t>
+  </si>
+  <si>
+    <t>Quality of life weights for different age groups</t>
+  </si>
+  <si>
+    <t>Life Tables for C11UK</t>
   </si>
 </sst>
 </file>
@@ -179,18 +221,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -473,108 +519,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.08984375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="20" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.08984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="2"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="93" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="G8" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C9"/>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="G7" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G8" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4" location="losExcelos "/>
+    <hyperlink ref="G9" r:id="rId5"/>
+    <hyperlink ref="G10" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some more references for the QOL studies
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eidennay\Documents\Other\general\covid19_QALY_calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eidennay\Documents\LSHTM\covid19\COVID19_QALY_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t xml:space="preserve">Access </t>
   </si>
@@ -145,9 +145,6 @@
     <t>https://www.canada.ca/content/dam/phac-aspc/documents/services/diseases/2019-novel-coronavirus-infection/surv-covid19-epi-update-eng.pdf</t>
   </si>
   <si>
-    <t>To be added</t>
-  </si>
-  <si>
     <t>CORONAVIRUS DISEASE 2019 (COVID-19) DAILY UPDATE</t>
   </si>
   <si>
@@ -164,6 +161,27 @@
   </si>
   <si>
     <t>Life Tables for C11UK</t>
+  </si>
+  <si>
+    <t>Xie F, Pullenayegum E, Gaebel K, Bansback N, Bryan S, Ohinmaa A, et al. A Time Trade-off-derived Value Set of the EQ-5D-5L for Canada. Med Care [Internet]. 2016 Jan;54(1):98–105. Available from: http://dx.doi.org/10.1097/MLR.0000000000000447</t>
+  </si>
+  <si>
+    <t>Open access manuscript</t>
+  </si>
+  <si>
+    <t>Janssen, B., &amp; Szende, A. (2014). Population norms for the EQ‐5D. Chapter 3. In A. Szende, B. Janssen, &amp; J. Cabases (Eds.), Self‐reported
+population health: An international perspective based on EQ‐5D. Amsterdam, Netherlands: Springer. 978‐94‐007‐7595‐4.</t>
+  </si>
+  <si>
+    <t>Open access report</t>
+  </si>
+  <si>
+    <t>Norwegian Medicines Agency. (2018). Guidelines for the submission of documentation for single technology assessment (STA) of pharmaceuticals
+[Internet]. Available from https://legemiddelverket.no/Documents/English/Public%20funding%20and%20pricing/
+Documentation%20for%20STA/Guidelines_april_2018.pdf</t>
+  </si>
+  <si>
+    <t>To be added - contact manuscript author</t>
   </si>
 </sst>
 </file>
@@ -522,7 +540,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -568,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
@@ -709,7 +727,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>26</v>
@@ -729,13 +747,13 @@
         <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -748,97 +766,97 @@
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>36</v>
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="174" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>